<commit_message>
I created the item list and their costs in advance
</commit_message>
<xml_diff>
--- a/Budget/Budget.xlsx
+++ b/Budget/Budget.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB0BDD38-1B49-40F3-83DD-9ECFAFA38FD2}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{034947AD-CB40-4343-9023-D9401C7D8E18}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -11,30 +11,27 @@
     <sheet name="Alinanlar" sheetId="1" r:id="rId1"/>
     <sheet name="Verilen Para" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="30">
   <si>
     <t>Adi Soyadi</t>
   </si>
   <si>
-    <t>Alinan</t>
-  </si>
-  <si>
-    <t>mouse</t>
-  </si>
-  <si>
-    <t>uzaklik sensoru</t>
-  </si>
-  <si>
     <t>Verdigi miktar</t>
   </si>
   <si>
@@ -59,25 +56,76 @@
     <t>19-25.11.18</t>
   </si>
   <si>
-    <t>Alinan Adet</t>
-  </si>
-  <si>
-    <t>Birim fiyati</t>
-  </si>
-  <si>
-    <t>Toplam Fiyat</t>
-  </si>
-  <si>
-    <t>Para Birimi</t>
-  </si>
-  <si>
-    <t>TL</t>
+    <t>Item Name</t>
+  </si>
+  <si>
+    <t>Nema17 Stepper Motor</t>
+  </si>
+  <si>
+    <t>Shipping Fee($)</t>
+  </si>
+  <si>
+    <t>Cost($)</t>
+  </si>
+  <si>
+    <t>Total($)</t>
+  </si>
+  <si>
+    <t>DRV8825 Stepper Motor Driver</t>
+  </si>
+  <si>
+    <t>TCA9548A IIC Expansion</t>
+  </si>
+  <si>
+    <t>Battery Charger Protection</t>
+  </si>
+  <si>
+    <t>PCF8574 GPIO Expander</t>
+  </si>
+  <si>
+    <t>5x VL53L0X</t>
+  </si>
+  <si>
+    <t>K783 Multi Hole Sheet</t>
+  </si>
+  <si>
+    <t>K836 Multi Hole Sheet</t>
+  </si>
+  <si>
+    <t>DS748 Stepper</t>
+  </si>
+  <si>
+    <t>28BYJ-48 Stepper and Expansion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2x VL6180X </t>
+  </si>
+  <si>
+    <t>Kale Padlock</t>
+  </si>
+  <si>
+    <t>VL53L0X From Turkey</t>
+  </si>
+  <si>
+    <t>70₺ in total</t>
+  </si>
+  <si>
+    <t>Trackball Mouse</t>
+  </si>
+  <si>
+    <t>J334 Shaft</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="6" formatCode="#,##0\ &quot;₺&quot;;[Red]\-#,##0\ &quot;₺&quot;"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -87,15 +135,33 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -103,12 +169,45 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -389,85 +488,594 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:E52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.5703125" customWidth="1"/>
-    <col min="2" max="2" width="26.7109375" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.140625" customWidth="1"/>
+    <col min="2" max="2" width="28.85546875" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" customWidth="1"/>
     <col min="5" max="5" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
+    <row r="1" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E1" t="s">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="3">
+        <v>1.1299999999999999</v>
+      </c>
+      <c r="C2" s="3">
+        <v>4.76</v>
+      </c>
+      <c r="D2" s="3">
+        <f t="shared" ref="D2" si="0">C2+B2</f>
+        <v>5.89</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F1" t="s">
+      <c r="B3" s="3">
+        <v>0</v>
+      </c>
+      <c r="C3" s="3">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D3" s="3">
+        <f t="shared" ref="D3:D51" si="1">C3+B3</f>
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2">
+      <c r="B4" s="3">
+        <v>0</v>
+      </c>
+      <c r="C4" s="3">
+        <v>1.06</v>
+      </c>
+      <c r="D4" s="3">
+        <f t="shared" si="1"/>
+        <v>1.06</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="3">
+        <v>0</v>
+      </c>
+      <c r="C5" s="3">
+        <v>1.0900000000000001</v>
+      </c>
+      <c r="D5" s="3">
+        <f t="shared" si="1"/>
+        <v>1.0900000000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="3">
+        <v>0</v>
+      </c>
+      <c r="C6" s="3">
+        <v>0.89</v>
+      </c>
+      <c r="D6" s="3">
+        <f t="shared" si="1"/>
+        <v>0.89</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="3">
+        <v>3.11</v>
+      </c>
+      <c r="C7" s="3">
+        <v>12.55</v>
+      </c>
+      <c r="D7" s="3">
+        <f t="shared" si="1"/>
+        <v>15.66</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="3">
+        <v>0</v>
+      </c>
+      <c r="C8" s="3">
+        <v>1.31</v>
+      </c>
+      <c r="D8" s="3">
+        <f t="shared" si="1"/>
+        <v>1.31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E2">
-        <v>20</v>
-      </c>
-      <c r="F2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3">
-        <v>70</v>
-      </c>
-      <c r="E3">
-        <v>70</v>
-      </c>
-      <c r="F3" t="s">
-        <v>16</v>
+      <c r="B9" s="3">
+        <v>0</v>
+      </c>
+      <c r="C9" s="3">
+        <v>0.82</v>
+      </c>
+      <c r="D9" s="3">
+        <f t="shared" si="1"/>
+        <v>0.82</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" s="3">
+        <v>0</v>
+      </c>
+      <c r="C10" s="3">
+        <v>1.04</v>
+      </c>
+      <c r="D10" s="3">
+        <f t="shared" si="1"/>
+        <v>1.04</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="3">
+        <v>0</v>
+      </c>
+      <c r="C11" s="3">
+        <v>1.53</v>
+      </c>
+      <c r="D11" s="3">
+        <f t="shared" si="1"/>
+        <v>1.53</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="3">
+        <v>0</v>
+      </c>
+      <c r="C12" s="3">
+        <v>1.28</v>
+      </c>
+      <c r="D12" s="3">
+        <f t="shared" si="1"/>
+        <v>1.28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="3">
+        <v>0</v>
+      </c>
+      <c r="C13" s="3">
+        <v>8.36</v>
+      </c>
+      <c r="D13" s="3">
+        <f t="shared" si="1"/>
+        <v>8.36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" s="3">
+        <v>0</v>
+      </c>
+      <c r="C14" s="3">
+        <v>5.99</v>
+      </c>
+      <c r="D14" s="3">
+        <f>C14+B14</f>
+        <v>5.99</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" s="3">
+        <v>1.26</v>
+      </c>
+      <c r="C15" s="3">
+        <v>12.35</v>
+      </c>
+      <c r="D15" s="3">
+        <f t="shared" si="1"/>
+        <v>13.61</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" s="3">
+        <v>0</v>
+      </c>
+      <c r="C16" s="3">
+        <v>3.8</v>
+      </c>
+      <c r="D16" s="3">
+        <f t="shared" si="1"/>
+        <v>3.8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="2"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="2"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="2"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="2"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="2"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="2"/>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="2"/>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="2"/>
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="2"/>
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="2"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="2"/>
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="2"/>
+      <c r="B28" s="3"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="2"/>
+      <c r="B29" s="3"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="2"/>
+      <c r="B30" s="3"/>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="2"/>
+      <c r="B31" s="3"/>
+      <c r="C31" s="3"/>
+      <c r="D31" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="2"/>
+      <c r="B32" s="3"/>
+      <c r="C32" s="3"/>
+      <c r="D32" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="2"/>
+      <c r="B33" s="3"/>
+      <c r="C33" s="3"/>
+      <c r="D33" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="2"/>
+      <c r="B34" s="3"/>
+      <c r="C34" s="3"/>
+      <c r="D34" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="2"/>
+      <c r="B35" s="3"/>
+      <c r="C35" s="3"/>
+      <c r="D35" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="2"/>
+      <c r="B36" s="3"/>
+      <c r="C36" s="3"/>
+      <c r="D36" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="2"/>
+      <c r="B37" s="3"/>
+      <c r="C37" s="3"/>
+      <c r="D37" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="2"/>
+      <c r="B38" s="3"/>
+      <c r="C38" s="3"/>
+      <c r="D38" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="2"/>
+      <c r="B39" s="3"/>
+      <c r="C39" s="3"/>
+      <c r="D39" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="2"/>
+      <c r="B40" s="3"/>
+      <c r="C40" s="3"/>
+      <c r="D40" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="2"/>
+      <c r="B41" s="3"/>
+      <c r="C41" s="3"/>
+      <c r="D41" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="2"/>
+      <c r="B42" s="3"/>
+      <c r="C42" s="3"/>
+      <c r="D42" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="2"/>
+      <c r="B43" s="3"/>
+      <c r="C43" s="3"/>
+      <c r="D43" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="2"/>
+      <c r="B44" s="3"/>
+      <c r="C44" s="3"/>
+      <c r="D44" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="2"/>
+      <c r="B45" s="3"/>
+      <c r="C45" s="3"/>
+      <c r="D45" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="2"/>
+      <c r="B46" s="3"/>
+      <c r="C46" s="3"/>
+      <c r="D46" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="2"/>
+      <c r="B47" s="3"/>
+      <c r="C47" s="3"/>
+      <c r="D47" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="2"/>
+      <c r="B48" s="3"/>
+      <c r="C48" s="3"/>
+      <c r="D48" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" s="2"/>
+      <c r="B49" s="3"/>
+      <c r="C49" s="3"/>
+      <c r="D49" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" s="2"/>
+      <c r="B50" s="3"/>
+      <c r="C50" s="3"/>
+      <c r="D50" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" s="2"/>
+      <c r="B51" s="3"/>
+      <c r="C51" s="3"/>
+      <c r="D51" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B52" s="4"/>
+      <c r="C52" s="4"/>
+      <c r="D52" s="6">
+        <f>SUM(D2:D51)</f>
+        <v>63.43</v>
+      </c>
+      <c r="E52" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -491,20 +1099,20 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C4">
         <v>100</v>
@@ -512,7 +1120,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C5">
         <v>100</v>
@@ -520,7 +1128,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C6">
         <v>100</v>
@@ -528,7 +1136,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C7">
         <v>100</v>
@@ -536,7 +1144,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C8">
         <v>100</v>

</xml_diff>

<commit_message>
I organize the budget chart
</commit_message>
<xml_diff>
--- a/Budget/Budget.xlsx
+++ b/Budget/Budget.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{034947AD-CB40-4343-9023-D9401C7D8E18}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C59BC72-5039-43FC-A0B2-6FBCA29EF747}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>Adi Soyadi</t>
   </si>
@@ -56,36 +56,21 @@
     <t>19-25.11.18</t>
   </si>
   <si>
-    <t>Item Name</t>
-  </si>
-  <si>
     <t>Nema17 Stepper Motor</t>
   </si>
   <si>
     <t>Shipping Fee($)</t>
   </si>
   <si>
-    <t>Cost($)</t>
-  </si>
-  <si>
-    <t>Total($)</t>
-  </si>
-  <si>
     <t>DRV8825 Stepper Motor Driver</t>
   </si>
   <si>
     <t>TCA9548A IIC Expansion</t>
   </si>
   <si>
-    <t>Battery Charger Protection</t>
-  </si>
-  <si>
     <t>PCF8574 GPIO Expander</t>
   </si>
   <si>
-    <t>5x VL53L0X</t>
-  </si>
-  <si>
     <t>K783 Multi Hole Sheet</t>
   </si>
   <si>
@@ -98,34 +83,43 @@
     <t>28BYJ-48 Stepper and Expansion</t>
   </si>
   <si>
-    <t xml:space="preserve">2x VL6180X </t>
-  </si>
-  <si>
     <t>Kale Padlock</t>
   </si>
   <si>
     <t>VL53L0X From Turkey</t>
   </si>
   <si>
-    <t>70₺ in total</t>
-  </si>
-  <si>
     <t>Trackball Mouse</t>
   </si>
   <si>
     <t>J334 Shaft</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
+    <t xml:space="preserve">Battery Protection Charger </t>
+  </si>
+  <si>
+    <t>Order Amount($)</t>
+  </si>
+  <si>
+    <t>Price per Unit($)</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VL6180X </t>
+  </si>
+  <si>
+    <t>VL53L0X</t>
+  </si>
+  <si>
+    <t>Item/Service  Name</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="6" formatCode="#,##0\ &quot;₺&quot;;[Red]\-#,##0\ &quot;₺&quot;"/>
-  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -202,11 +196,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -490,587 +484,662 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="32.140625" customWidth="1"/>
-    <col min="2" max="2" width="28.85546875" customWidth="1"/>
-    <col min="3" max="3" width="14.7109375" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" customWidth="1"/>
-    <col min="5" max="5" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" customWidth="1"/>
+    <col min="4" max="4" width="16.85546875" customWidth="1"/>
+    <col min="5" max="5" width="18" customWidth="1"/>
+    <col min="6" max="6" width="19.85546875" customWidth="1"/>
+    <col min="7" max="7" width="20.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>13</v>
+        <v>24</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B2" s="3">
+        <v>18</v>
+      </c>
+      <c r="B2" s="6">
+        <v>1</v>
+      </c>
+      <c r="C2" s="3">
         <v>1.1299999999999999</v>
       </c>
-      <c r="C2" s="3">
+      <c r="D2" s="3">
         <v>4.76</v>
       </c>
-      <c r="D2" s="3">
-        <f t="shared" ref="D2" si="0">C2+B2</f>
+      <c r="E2" s="3">
+        <f>C2+B2*D2</f>
         <v>5.89</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" s="3">
-        <v>0</v>
+        <v>11</v>
+      </c>
+      <c r="B3" s="6">
+        <v>1</v>
       </c>
       <c r="C3" s="3">
+        <v>0</v>
+      </c>
+      <c r="D3" s="3">
         <v>1.1000000000000001</v>
       </c>
-      <c r="D3" s="3">
-        <f t="shared" ref="D3:D51" si="1">C3+B3</f>
+      <c r="E3" s="3">
+        <f t="shared" ref="E3:E51" si="0">C3+B3*D3</f>
         <v>1.1000000000000001</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" s="3">
-        <v>0</v>
+        <v>12</v>
+      </c>
+      <c r="B4" s="6">
+        <v>1</v>
       </c>
       <c r="C4" s="3">
+        <v>0</v>
+      </c>
+      <c r="D4" s="3">
         <v>1.06</v>
       </c>
-      <c r="D4" s="3">
-        <f t="shared" si="1"/>
+      <c r="E4" s="3">
+        <f t="shared" si="0"/>
         <v>1.06</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" s="3">
-        <v>0</v>
+        <v>22</v>
+      </c>
+      <c r="B5" s="6">
+        <v>1</v>
       </c>
       <c r="C5" s="3">
+        <v>0</v>
+      </c>
+      <c r="D5" s="3">
         <v>1.0900000000000001</v>
       </c>
-      <c r="D5" s="3">
-        <f t="shared" si="1"/>
+      <c r="E5" s="3">
+        <f t="shared" si="0"/>
         <v>1.0900000000000001</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" s="3">
-        <v>0</v>
+        <v>13</v>
+      </c>
+      <c r="B6" s="6">
+        <v>1</v>
       </c>
       <c r="C6" s="3">
+        <v>0</v>
+      </c>
+      <c r="D6" s="3">
         <v>0.89</v>
       </c>
-      <c r="D6" s="3">
-        <f t="shared" si="1"/>
+      <c r="E6" s="3">
+        <f t="shared" si="0"/>
         <v>0.89</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" s="3">
+        <v>27</v>
+      </c>
+      <c r="B7" s="6">
+        <v>5</v>
+      </c>
+      <c r="C7" s="3">
         <v>3.11</v>
       </c>
-      <c r="C7" s="3">
-        <v>12.55</v>
-      </c>
       <c r="D7" s="3">
-        <f t="shared" si="1"/>
-        <v>15.66</v>
+        <v>2.5099999999999998</v>
+      </c>
+      <c r="E7" s="3">
+        <f t="shared" si="0"/>
+        <v>15.659999999999998</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B8" s="3">
-        <v>0</v>
+        <v>14</v>
+      </c>
+      <c r="B8" s="6">
+        <v>1</v>
       </c>
       <c r="C8" s="3">
+        <v>0</v>
+      </c>
+      <c r="D8" s="3">
         <v>1.31</v>
       </c>
-      <c r="D8" s="3">
-        <f t="shared" si="1"/>
+      <c r="E8" s="3">
+        <f t="shared" si="0"/>
         <v>1.31</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B9" s="3">
-        <v>0</v>
+        <v>15</v>
+      </c>
+      <c r="B9" s="6">
+        <v>1</v>
       </c>
       <c r="C9" s="3">
+        <v>0</v>
+      </c>
+      <c r="D9" s="3">
         <v>0.82</v>
       </c>
-      <c r="D9" s="3">
-        <f t="shared" si="1"/>
+      <c r="E9" s="3">
+        <f t="shared" si="0"/>
         <v>0.82</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B10" s="3">
-        <v>0</v>
+        <v>21</v>
+      </c>
+      <c r="B10" s="6">
+        <v>1</v>
       </c>
       <c r="C10" s="3">
+        <v>0</v>
+      </c>
+      <c r="D10" s="3">
         <v>1.04</v>
       </c>
-      <c r="D10" s="3">
-        <f t="shared" si="1"/>
+      <c r="E10" s="3">
+        <f t="shared" si="0"/>
         <v>1.04</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B11" s="3">
-        <v>0</v>
+        <v>16</v>
+      </c>
+      <c r="B11" s="6">
+        <v>1</v>
       </c>
       <c r="C11" s="3">
+        <v>0</v>
+      </c>
+      <c r="D11" s="3">
         <v>1.53</v>
       </c>
-      <c r="D11" s="3">
-        <f t="shared" si="1"/>
+      <c r="E11" s="3">
+        <f t="shared" si="0"/>
         <v>1.53</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B12" s="3">
-        <v>0</v>
+        <v>17</v>
+      </c>
+      <c r="B12" s="6">
+        <v>1</v>
       </c>
       <c r="C12" s="3">
+        <v>0</v>
+      </c>
+      <c r="D12" s="3">
         <v>1.28</v>
       </c>
-      <c r="D12" s="3">
-        <f t="shared" si="1"/>
+      <c r="E12" s="3">
+        <f t="shared" si="0"/>
         <v>1.28</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B13" s="3">
-        <v>0</v>
+        <v>26</v>
+      </c>
+      <c r="B13" s="6">
+        <v>2</v>
       </c>
       <c r="C13" s="3">
-        <v>8.36</v>
+        <v>0</v>
       </c>
       <c r="D13" s="3">
-        <f t="shared" si="1"/>
+        <v>4.18</v>
+      </c>
+      <c r="E13" s="3">
+        <f t="shared" si="0"/>
         <v>8.36</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B14" s="3">
-        <v>0</v>
+        <v>9</v>
+      </c>
+      <c r="B14" s="6">
+        <v>1</v>
       </c>
       <c r="C14" s="3">
+        <v>0</v>
+      </c>
+      <c r="D14" s="3">
         <v>5.99</v>
       </c>
-      <c r="D14" s="3">
-        <f>C14+B14</f>
+      <c r="E14" s="3">
+        <f t="shared" si="0"/>
         <v>5.99</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B15" s="3">
+        <v>19</v>
+      </c>
+      <c r="B15" s="6">
+        <v>1</v>
+      </c>
+      <c r="C15" s="3">
         <v>1.26</v>
       </c>
-      <c r="C15" s="3">
+      <c r="D15" s="3">
         <v>12.35</v>
       </c>
-      <c r="D15" s="3">
-        <f t="shared" si="1"/>
+      <c r="E15" s="3">
+        <f t="shared" si="0"/>
         <v>13.61</v>
-      </c>
-      <c r="E15" s="5" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B16" s="3">
-        <v>0</v>
+        <v>20</v>
+      </c>
+      <c r="B16" s="6">
+        <v>1</v>
       </c>
       <c r="C16" s="3">
+        <v>0</v>
+      </c>
+      <c r="D16" s="3">
         <v>3.8</v>
       </c>
-      <c r="D16" s="3">
-        <f t="shared" si="1"/>
+      <c r="E16" s="3">
+        <f t="shared" si="0"/>
         <v>3.8</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
-      <c r="B17" s="3"/>
+      <c r="B17" s="6"/>
       <c r="C17" s="3"/>
-      <c r="D17" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D17" s="3"/>
+      <c r="E17" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
-      <c r="B18" s="3"/>
+      <c r="B18" s="6"/>
       <c r="C18" s="3"/>
-      <c r="D18" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D18" s="3"/>
+      <c r="E18" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
-      <c r="B19" s="3"/>
+      <c r="B19" s="6"/>
       <c r="C19" s="3"/>
-      <c r="D19" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D19" s="3"/>
+      <c r="E19" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
-      <c r="B20" s="3"/>
+      <c r="B20" s="6"/>
       <c r="C20" s="3"/>
-      <c r="D20" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D20" s="3"/>
+      <c r="E20" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
-      <c r="B21" s="3"/>
+      <c r="B21" s="6"/>
       <c r="C21" s="3"/>
-      <c r="D21" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D21" s="3"/>
+      <c r="E21" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
-      <c r="B22" s="3"/>
+      <c r="B22" s="6"/>
       <c r="C22" s="3"/>
-      <c r="D22" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D22" s="3"/>
+      <c r="E22" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
-      <c r="B23" s="3"/>
+      <c r="B23" s="6"/>
       <c r="C23" s="3"/>
-      <c r="D23" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D23" s="3"/>
+      <c r="E23" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
-      <c r="B24" s="3"/>
+      <c r="B24" s="6"/>
       <c r="C24" s="3"/>
-      <c r="D24" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D24" s="3"/>
+      <c r="E24" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
-      <c r="B25" s="3"/>
+      <c r="B25" s="6"/>
       <c r="C25" s="3"/>
-      <c r="D25" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D25" s="3"/>
+      <c r="E25" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
-      <c r="B26" s="3"/>
+      <c r="B26" s="6"/>
       <c r="C26" s="3"/>
-      <c r="D26" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D26" s="3"/>
+      <c r="E26" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
-      <c r="B27" s="3"/>
+      <c r="B27" s="6"/>
       <c r="C27" s="3"/>
-      <c r="D27" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D27" s="3"/>
+      <c r="E27" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
-      <c r="B28" s="3"/>
+      <c r="B28" s="6"/>
       <c r="C28" s="3"/>
-      <c r="D28" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D28" s="3"/>
+      <c r="E28" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
-      <c r="B29" s="3"/>
+      <c r="B29" s="6"/>
       <c r="C29" s="3"/>
-      <c r="D29" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D29" s="3"/>
+      <c r="E29" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
-      <c r="B30" s="3"/>
+      <c r="B30" s="6"/>
       <c r="C30" s="3"/>
-      <c r="D30" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D30" s="3"/>
+      <c r="E30" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="2"/>
-      <c r="B31" s="3"/>
+      <c r="B31" s="6"/>
       <c r="C31" s="3"/>
-      <c r="D31" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D31" s="3"/>
+      <c r="E31" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="2"/>
-      <c r="B32" s="3"/>
+      <c r="B32" s="6"/>
       <c r="C32" s="3"/>
-      <c r="D32" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D32" s="3"/>
+      <c r="E32" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="2"/>
-      <c r="B33" s="3"/>
+      <c r="B33" s="6"/>
       <c r="C33" s="3"/>
-      <c r="D33" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D33" s="3"/>
+      <c r="E33" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="2"/>
-      <c r="B34" s="3"/>
+      <c r="B34" s="6"/>
       <c r="C34" s="3"/>
-      <c r="D34" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D34" s="3"/>
+      <c r="E34" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="2"/>
-      <c r="B35" s="3"/>
+      <c r="B35" s="6"/>
       <c r="C35" s="3"/>
-      <c r="D35" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D35" s="3"/>
+      <c r="E35" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="2"/>
-      <c r="B36" s="3"/>
+      <c r="B36" s="6"/>
       <c r="C36" s="3"/>
-      <c r="D36" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D36" s="3"/>
+      <c r="E36" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="2"/>
-      <c r="B37" s="3"/>
+      <c r="B37" s="6"/>
       <c r="C37" s="3"/>
-      <c r="D37" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D37" s="3"/>
+      <c r="E37" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="2"/>
-      <c r="B38" s="3"/>
+      <c r="B38" s="6"/>
       <c r="C38" s="3"/>
-      <c r="D38" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D38" s="3"/>
+      <c r="E38" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="2"/>
-      <c r="B39" s="3"/>
+      <c r="B39" s="6"/>
       <c r="C39" s="3"/>
-      <c r="D39" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D39" s="3"/>
+      <c r="E39" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="2"/>
-      <c r="B40" s="3"/>
+      <c r="B40" s="6"/>
       <c r="C40" s="3"/>
-      <c r="D40" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D40" s="3"/>
+      <c r="E40" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="2"/>
-      <c r="B41" s="3"/>
+      <c r="B41" s="6"/>
       <c r="C41" s="3"/>
-      <c r="D41" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D41" s="3"/>
+      <c r="E41" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="2"/>
-      <c r="B42" s="3"/>
+      <c r="B42" s="6"/>
       <c r="C42" s="3"/>
-      <c r="D42" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D42" s="3"/>
+      <c r="E42" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="2"/>
-      <c r="B43" s="3"/>
+      <c r="B43" s="6"/>
       <c r="C43" s="3"/>
-      <c r="D43" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D43" s="3"/>
+      <c r="E43" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="2"/>
-      <c r="B44" s="3"/>
+      <c r="B44" s="6"/>
       <c r="C44" s="3"/>
-      <c r="D44" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D44" s="3"/>
+      <c r="E44" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="2"/>
-      <c r="B45" s="3"/>
+      <c r="B45" s="6"/>
       <c r="C45" s="3"/>
-      <c r="D45" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D45" s="3"/>
+      <c r="E45" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="2"/>
-      <c r="B46" s="3"/>
+      <c r="B46" s="6"/>
       <c r="C46" s="3"/>
-      <c r="D46" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D46" s="3"/>
+      <c r="E46" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="2"/>
-      <c r="B47" s="3"/>
+      <c r="B47" s="6"/>
       <c r="C47" s="3"/>
-      <c r="D47" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D47" s="3"/>
+      <c r="E47" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="2"/>
-      <c r="B48" s="3"/>
+      <c r="B48" s="6"/>
       <c r="C48" s="3"/>
-      <c r="D48" s="3">
-        <f t="shared" si="1"/>
+      <c r="D48" s="3"/>
+      <c r="E48" s="3">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="2"/>
-      <c r="B49" s="3"/>
+      <c r="B49" s="6"/>
       <c r="C49" s="3"/>
-      <c r="D49" s="3">
-        <f t="shared" si="1"/>
+      <c r="D49" s="3"/>
+      <c r="E49" s="3">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="2"/>
-      <c r="B50" s="3"/>
+      <c r="B50" s="6"/>
       <c r="C50" s="3"/>
-      <c r="D50" s="3">
-        <f t="shared" si="1"/>
+      <c r="D50" s="3"/>
+      <c r="E50" s="3">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="2"/>
-      <c r="B51" s="3"/>
+      <c r="B51" s="6"/>
       <c r="C51" s="3"/>
-      <c r="D51" s="3">
-        <f t="shared" si="1"/>
+      <c r="D51" s="3"/>
+      <c r="E51" s="3">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B52" s="4"/>
       <c r="C52" s="4"/>
-      <c r="D52" s="6">
-        <f>SUM(D2:D51)</f>
+      <c r="D52" s="4"/>
+      <c r="E52" s="5">
+        <f>SUM(E2:E51)</f>
         <v>63.43</v>
-      </c>
-      <c r="E52" t="s">
-        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
I updated the budget list
</commit_message>
<xml_diff>
--- a/Budget/Budget.xlsx
+++ b/Budget/Budget.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C59BC72-5039-43FC-A0B2-6FBCA29EF747}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA2039ED-DADC-4923-BBEE-406F83B8EA80}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>Adi Soyadi</t>
   </si>
@@ -114,6 +114,24 @@
   </si>
   <si>
     <t>Item/Service  Name</t>
+  </si>
+  <si>
+    <t>L298N</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TB6612FNG </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.91" white/Blue OLED </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> GY-273  HMC5883L</t>
+  </si>
+  <si>
+    <t>MEGA2560</t>
+  </si>
+  <si>
+    <t>TP5100</t>
   </si>
 </sst>
 </file>
@@ -484,7 +502,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -785,63 +805,111 @@
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="2"/>
-      <c r="B17" s="6"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
+      <c r="A17" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B17" s="6">
+        <v>1</v>
+      </c>
+      <c r="C17" s="3">
+        <v>0</v>
+      </c>
+      <c r="D17" s="3">
+        <v>0.44</v>
+      </c>
       <c r="E17" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.44</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="2"/>
-      <c r="B18" s="6"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
+      <c r="A18" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B18" s="6">
+        <v>1</v>
+      </c>
+      <c r="C18" s="3">
+        <v>0</v>
+      </c>
+      <c r="D18" s="3">
+        <v>1.0900000000000001</v>
+      </c>
       <c r="E18" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.0900000000000001</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="2"/>
-      <c r="B19" s="6"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
+      <c r="A19" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B19" s="6">
+        <v>1</v>
+      </c>
+      <c r="C19" s="3">
+        <v>0</v>
+      </c>
+      <c r="D19" s="3">
+        <v>1.56</v>
+      </c>
       <c r="E19" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.56</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="2"/>
-      <c r="B20" s="6"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
+      <c r="A20" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B20" s="6">
+        <v>1</v>
+      </c>
+      <c r="C20" s="3">
+        <v>0</v>
+      </c>
+      <c r="D20" s="3">
+        <v>1.82</v>
+      </c>
       <c r="E20" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.82</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="2"/>
-      <c r="B21" s="6"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
+      <c r="A21" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B21" s="6">
+        <v>1</v>
+      </c>
+      <c r="C21" s="3">
+        <v>2.11</v>
+      </c>
+      <c r="D21" s="3">
+        <v>7.95</v>
+      </c>
       <c r="E21" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>10.06</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="2"/>
-      <c r="B22" s="6"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
+      <c r="A22" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B22" s="6">
+        <v>1</v>
+      </c>
+      <c r="C22" s="3">
+        <v>0</v>
+      </c>
+      <c r="D22" s="3">
+        <v>0.61</v>
+      </c>
       <c r="E22" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.61</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -1139,7 +1207,7 @@
       <c r="D52" s="4"/>
       <c r="E52" s="5">
         <f>SUM(E2:E51)</f>
-        <v>63.43</v>
+        <v>79.009999999999991</v>
       </c>
     </row>
   </sheetData>

</xml_diff>